<commit_message>
Bug fix: handle date like 'midMarch'
</commit_message>
<xml_diff>
--- a/DECS Excel Add-Ins/test files/time parsing.xlsx
+++ b/DECS Excel Add-Ins/test files/time parsing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\DECS-Office-AddIns\DECS Excel Add-Ins\test files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{215B63B6-9F77-4174-ABCF-CF77D3F7953C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A226FE0D-319E-48C4-B414-2B98CE145273}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{29FD6E34-14AD-42F4-982A-2D09B34F1C51}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Note written</t>
   </si>
@@ -133,6 +133,9 @@
   </si>
   <si>
     <t>June/July</t>
+  </si>
+  <si>
+    <t>midMarch 2025</t>
   </si>
 </sst>
 </file>
@@ -186,7 +189,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -194,23 +197,16 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="CenteredHeadings" xfId="1" xr:uid="{9C049AE3-3089-4AA6-A275-DA14C403F95F}"/>
@@ -526,11 +522,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CA9BBE-1EDE-4111-809C-59966F94183B}">
-  <dimension ref="A1:B42"/>
+  <dimension ref="A1:B43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -543,7 +539,7 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
     </row>
@@ -579,236 +575,236 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="15">
+    <row r="6" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
         <v>45468.642361111109</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>45468.696527777778</v>
+    <row r="7" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
+        <v>45468.642361111109</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>45468.696527777778</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
-        <v>45468.597916666666</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
-        <v>45468.599305555559</v>
+        <v>45468.597916666666</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
-        <v>45468.618055555555</v>
-      </c>
-      <c r="B10" s="6">
-        <v>45513</v>
+        <v>45468.599305555559</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
-        <v>45468.642361111109</v>
-      </c>
-      <c r="B11" s="7">
-        <v>45627</v>
+        <v>45468.618055555555</v>
+      </c>
+      <c r="B11" s="5">
+        <v>45513</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
-        <v>45468.696527777778</v>
-      </c>
-      <c r="B12" s="7">
-        <v>45597</v>
+        <v>45468.642361111109</v>
+      </c>
+      <c r="B12" s="5">
+        <v>45627</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
-        <v>45468.597916666666</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>9</v>
+        <v>45468.696527777778</v>
+      </c>
+      <c r="B13" s="5">
+        <v>45597</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
-        <v>45468.599305555559</v>
-      </c>
-      <c r="B14" s="7">
-        <v>45839</v>
+        <v>45468.597916666666</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
-        <v>45468.618055555555</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>10</v>
+        <v>45468.599305555559</v>
+      </c>
+      <c r="B15" s="5">
+        <v>45839</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
-        <v>45468.642361111109</v>
+        <v>45468.618055555555</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
-        <v>45468.696527777778</v>
-      </c>
-      <c r="B17" s="7">
-        <v>45689</v>
+        <v>45468.642361111109</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
-        <v>45468.597916666666</v>
-      </c>
-      <c r="B18" s="7">
-        <v>45717</v>
+        <v>45468.696527777778</v>
+      </c>
+      <c r="B18" s="5">
+        <v>45689</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
-        <v>45468.599305555559</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>27</v>
+        <v>45468.597916666666</v>
+      </c>
+      <c r="B19" s="5">
+        <v>45717</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
-        <v>45468.618055555555</v>
+        <v>45468.599305555559</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
-        <v>45468.642361111109</v>
-      </c>
-      <c r="B21" s="7">
-        <v>45962</v>
+        <v>45468.618055555555</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
-        <v>45468.696527777778</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>13</v>
+        <v>45468.642361111109</v>
+      </c>
+      <c r="B22" s="5">
+        <v>45962</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
-        <v>45468.597916666666</v>
+        <v>45468.696527777778</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
-        <v>45468.599305555559</v>
+        <v>45468.597916666666</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
-        <v>45468.618055555555</v>
+        <v>45468.599305555559</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
-        <v>45468.642361111109</v>
+        <v>45468.618055555555</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
-        <v>45468.696527777778</v>
+        <v>45468.642361111109</v>
       </c>
       <c r="B27" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="3">
+        <v>45468.696527777778</v>
+      </c>
+      <c r="B28" s="5" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="4">
-        <v>45468.642361111109</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
-        <v>45468.696527777778</v>
+        <v>45468.642361111109</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
-        <v>45468.597916666666</v>
+        <v>45468.696527777778</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
-        <v>45468.599305555559</v>
+        <v>45468.597916666666</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
-        <v>45468.618055555555</v>
+        <v>45468.599305555559</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
-        <v>45468.642361111109</v>
+        <v>45468.618055555555</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
-        <v>45468.696527777778</v>
+        <v>45468.642361111109</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -816,62 +812,70 @@
         <v>45468.696527777778</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
-        <v>45468.597916666666</v>
-      </c>
-      <c r="B36" s="8" t="s">
-        <v>28</v>
+        <v>45468.696527777778</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
-        <v>45468.599305555559</v>
-      </c>
-      <c r="B37" s="9" t="s">
-        <v>29</v>
+        <v>45468.597916666666</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
-        <v>45468.618055555555</v>
+        <v>45468.599305555559</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
-        <v>45468.642361111109</v>
-      </c>
-      <c r="B39" s="11" t="s">
-        <v>31</v>
+        <v>45468.618055555555</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
-        <v>45468.696527777778</v>
-      </c>
-      <c r="B40" s="12" t="s">
+        <v>45468.642361111109</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="4">
+        <v>45468.696527777778</v>
+      </c>
+      <c r="B41" s="10" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="13">
-        <v>45468.696527777778</v>
-      </c>
-      <c r="B41" s="12" t="s">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="6">
+        <v>45468.696527777778</v>
+      </c>
+      <c r="B42" s="10" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="15">
-        <v>45468.642361111109</v>
-      </c>
-      <c r="B42" s="14" t="s">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="8">
+        <v>45468.642361111109</v>
+      </c>
+      <c r="B43" s="10" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>